<commit_message>
finalized pipeline sans forecasting section
</commit_message>
<xml_diff>
--- a/may-pipeline/optimized_month.xlsx
+++ b/may-pipeline/optimized_month.xlsx
@@ -419,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,52 +480,52 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1176.733931728567</v>
+        <v>388.3352901922048</v>
       </c>
       <c r="C2">
-        <v>1017.932519871152</v>
+        <v>446.2195923665384</v>
       </c>
       <c r="D2">
-        <v>69.15332955993401</v>
+        <v>796.8717088444853</v>
       </c>
       <c r="E2">
-        <v>767.5446540156451</v>
+        <v>1223.667152204717</v>
       </c>
       <c r="F2">
-        <v>535.805880082381</v>
+        <v>658.7459749266949</v>
       </c>
       <c r="G2">
-        <v>753.9915445720669</v>
+        <v>976.538585599327</v>
       </c>
       <c r="H2">
-        <v>694.502914572222</v>
+        <v>45.96927808875708</v>
       </c>
       <c r="I2">
-        <v>904.1914901693325</v>
+        <v>207.6241154558886</v>
       </c>
       <c r="J2">
-        <v>423.6522445697167</v>
+        <v>207.344928223961</v>
       </c>
       <c r="K2">
-        <v>486.5957209239945</v>
+        <v>145.0241895788428</v>
       </c>
       <c r="L2">
-        <v>1027.37813391103</v>
+        <v>1086.219478593982</v>
       </c>
       <c r="M2">
-        <v>768.1288448600235</v>
+        <v>683.9517667123285</v>
       </c>
       <c r="N2">
-        <v>869.5130071128877</v>
+        <v>1102.932997314316</v>
       </c>
       <c r="O2">
-        <v>628.3066649646937</v>
+        <v>368.5470637799975</v>
       </c>
       <c r="P2">
-        <v>134.8431858082247</v>
+        <v>113.3158109211705</v>
       </c>
       <c r="Q2">
-        <v>219.661212507058</v>
+        <v>1158.335535610222</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -533,52 +533,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1106.330326007158</v>
+        <v>430.4411774077913</v>
       </c>
       <c r="C3">
-        <v>118.4994596510207</v>
+        <v>1167.015708192014</v>
       </c>
       <c r="D3">
-        <v>962.5629107052735</v>
+        <v>709.6106127082278</v>
       </c>
       <c r="E3">
-        <v>597.3602998795606</v>
+        <v>905.8618419258008</v>
       </c>
       <c r="F3">
-        <v>370.8139249075174</v>
+        <v>228.0960420590512</v>
       </c>
       <c r="G3">
-        <v>1056.59336470459</v>
+        <v>1193.38948844447</v>
       </c>
       <c r="H3">
-        <v>847.7694661986799</v>
+        <v>1103.455202303821</v>
       </c>
       <c r="I3">
-        <v>685.3110281916265</v>
+        <v>1144.226645563802</v>
       </c>
       <c r="J3">
-        <v>1064.228185722834</v>
+        <v>461.9086477336938</v>
       </c>
       <c r="K3">
-        <v>836.159574720731</v>
+        <v>914.8943780097393</v>
       </c>
       <c r="L3">
-        <v>781.5885686171155</v>
+        <v>1033.239357276007</v>
       </c>
       <c r="M3">
-        <v>727.3042820570413</v>
+        <v>664.3256268626874</v>
       </c>
       <c r="N3">
-        <v>446.1638128152738</v>
+        <v>336.2102315110374</v>
       </c>
       <c r="O3">
-        <v>991.3091329360828</v>
+        <v>358.4263530350149</v>
       </c>
       <c r="P3">
-        <v>52.11609116766998</v>
+        <v>1097.717566967331</v>
       </c>
       <c r="Q3">
-        <v>1176.760386360995</v>
+        <v>415.8958860834792</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -586,52 +586,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>317.4265375794598</v>
+        <v>909.434089185743</v>
       </c>
       <c r="C4">
-        <v>981.9810192055078</v>
+        <v>535.4594072400191</v>
       </c>
       <c r="D4">
-        <v>984.4652106156798</v>
+        <v>610.962717591707</v>
       </c>
       <c r="E4">
-        <v>762.358019292251</v>
+        <v>530.255708590965</v>
       </c>
       <c r="F4">
-        <v>1186.709750443262</v>
+        <v>348.4650675481665</v>
       </c>
       <c r="G4">
-        <v>782.1734573776974</v>
+        <v>1019.097262704726</v>
       </c>
       <c r="H4">
-        <v>244.6943487000351</v>
+        <v>9.961855897162447</v>
       </c>
       <c r="I4">
-        <v>1151.428410807204</v>
+        <v>564.6119322170946</v>
       </c>
       <c r="J4">
-        <v>399.1876991104448</v>
+        <v>1073.906976342059</v>
       </c>
       <c r="K4">
-        <v>733.3531096164817</v>
+        <v>92.74360851709986</v>
       </c>
       <c r="L4">
-        <v>139.7091919739887</v>
+        <v>843.2670553873922</v>
       </c>
       <c r="M4">
-        <v>334.4567877936195</v>
+        <v>829.8830852313483</v>
       </c>
       <c r="N4">
-        <v>533.5012735794843</v>
+        <v>1247.855771548336</v>
       </c>
       <c r="O4">
-        <v>112.7336765355803</v>
+        <v>60.40322310668693</v>
       </c>
       <c r="P4">
-        <v>588.8410557943372</v>
+        <v>711.732205411163</v>
       </c>
       <c r="Q4">
-        <v>1009.352440391386</v>
+        <v>244.8397638193451</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -639,52 +639,52 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>103.4697193303798</v>
+        <v>1020.342546528575</v>
       </c>
       <c r="C5">
-        <v>823.1201493903529</v>
+        <v>337.3996854308602</v>
       </c>
       <c r="D5">
-        <v>104.8888429993506</v>
+        <v>1122.804312318031</v>
       </c>
       <c r="E5">
-        <v>1208.5446943232</v>
+        <v>943.8016348041735</v>
       </c>
       <c r="F5">
-        <v>954.4666714748224</v>
+        <v>1020.943758012779</v>
       </c>
       <c r="G5">
-        <v>42.36405127065913</v>
+        <v>472.7900792568786</v>
       </c>
       <c r="H5">
-        <v>84.36873218488574</v>
+        <v>739.2607524292813</v>
       </c>
       <c r="I5">
-        <v>756.4893581818371</v>
+        <v>117.5988046176906</v>
       </c>
       <c r="J5">
-        <v>45.00068530407229</v>
+        <v>18.0897440207971</v>
       </c>
       <c r="K5">
-        <v>694.1569896635809</v>
+        <v>1113.227123779788</v>
       </c>
       <c r="L5">
-        <v>855.9849457028871</v>
+        <v>526.615784020447</v>
       </c>
       <c r="M5">
-        <v>688.0862497697372</v>
+        <v>176.0192409548637</v>
       </c>
       <c r="N5">
-        <v>310.759317547415</v>
+        <v>428.5529880320795</v>
       </c>
       <c r="O5">
-        <v>141.7062367339911</v>
+        <v>621.418993770444</v>
       </c>
       <c r="P5">
-        <v>1088.053740333036</v>
+        <v>421.7060494421864</v>
       </c>
       <c r="Q5">
-        <v>289.852163169416</v>
+        <v>124.2081091842892</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -692,317 +692,52 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>142.4898700560503</v>
+        <v>478.7709662241166</v>
       </c>
       <c r="C6">
-        <v>549.311714603293</v>
+        <v>353.2117471623208</v>
       </c>
       <c r="D6">
-        <v>1187.083180206441</v>
+        <v>680.0767837199633</v>
       </c>
       <c r="E6">
-        <v>820.8289371909927</v>
+        <v>630.8885166157535</v>
       </c>
       <c r="F6">
-        <v>1049.247936323138</v>
+        <v>511.148213610521</v>
       </c>
       <c r="G6">
-        <v>896.3555878868532</v>
+        <v>999.2494999471149</v>
       </c>
       <c r="H6">
-        <v>1166.543196220167</v>
+        <v>586.7084529148684</v>
       </c>
       <c r="I6">
-        <v>474.7469817537133</v>
+        <v>746.7335110676952</v>
       </c>
       <c r="J6">
-        <v>153.5474749375532</v>
+        <v>562.7050077563615</v>
       </c>
       <c r="K6">
-        <v>944.4604836624898</v>
+        <v>947.2757186363422</v>
       </c>
       <c r="L6">
-        <v>228.2101790704702</v>
+        <v>882.7140165453911</v>
       </c>
       <c r="M6">
-        <v>321.4185125980085</v>
+        <v>214.5415964105117</v>
       </c>
       <c r="N6">
-        <v>853.7460919779727</v>
+        <v>837.8539801295253</v>
       </c>
       <c r="O6">
-        <v>902.4191495524271</v>
+        <v>389.0422575903189</v>
       </c>
       <c r="P6">
-        <v>214.2158306925529</v>
+        <v>257.3824980285746</v>
       </c>
       <c r="Q6">
-        <v>566.6434947188552</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>576.8679303302542</v>
-      </c>
-      <c r="C7">
-        <v>230.1644109207452</v>
-      </c>
-      <c r="D7">
-        <v>722.9285150069712</v>
-      </c>
-      <c r="E7">
-        <v>3.291444191131182</v>
-      </c>
-      <c r="F7">
-        <v>269.994571665293</v>
-      </c>
-      <c r="G7">
-        <v>1162.126442876565</v>
-      </c>
-      <c r="H7">
-        <v>513.6873225702528</v>
-      </c>
-      <c r="I7">
-        <v>888.648924461011</v>
-      </c>
-      <c r="J7">
-        <v>40.19112407535668</v>
-      </c>
-      <c r="K7">
-        <v>455.4697647893197</v>
-      </c>
-      <c r="L7">
-        <v>507.8166585178708</v>
-      </c>
-      <c r="M7">
-        <v>274.6898365358354</v>
-      </c>
-      <c r="N7">
-        <v>617.0747590649859</v>
-      </c>
-      <c r="O7">
-        <v>776.8181804167507</v>
-      </c>
-      <c r="P7">
-        <v>46.78842811015595</v>
-      </c>
-      <c r="Q7">
-        <v>1213.7901288832</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>254.4346693634459</v>
-      </c>
-      <c r="C8">
-        <v>756.8997981771931</v>
-      </c>
-      <c r="D8">
-        <v>491.4827114040858</v>
-      </c>
-      <c r="E8">
-        <v>644.5689783775025</v>
-      </c>
-      <c r="F8">
-        <v>782.9144826570197</v>
-      </c>
-      <c r="G8">
-        <v>1029.210457719157</v>
-      </c>
-      <c r="H8">
-        <v>432.2517133559603</v>
-      </c>
-      <c r="I8">
-        <v>204.9849876486489</v>
-      </c>
-      <c r="J8">
-        <v>270.1263834833546</v>
-      </c>
-      <c r="K8">
-        <v>630.7341397907433</v>
-      </c>
-      <c r="L8">
-        <v>1067.068036442127</v>
-      </c>
-      <c r="M8">
-        <v>967.2970087056627</v>
-      </c>
-      <c r="N8">
-        <v>1233.006467938278</v>
-      </c>
-      <c r="O8">
-        <v>249.2930945759052</v>
-      </c>
-      <c r="P8">
-        <v>1172.179383122898</v>
-      </c>
-      <c r="Q8">
-        <v>199.3159165965801</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>782.1100604569164</v>
-      </c>
-      <c r="C9">
-        <v>182.6309052004176</v>
-      </c>
-      <c r="D9">
-        <v>771.2646405973805</v>
-      </c>
-      <c r="E9">
-        <v>1069.645425054642</v>
-      </c>
-      <c r="F9">
-        <v>8.265809744875764</v>
-      </c>
-      <c r="G9">
-        <v>1108.71389353229</v>
-      </c>
-      <c r="H9">
-        <v>808.935497575618</v>
-      </c>
-      <c r="I9">
-        <v>1095.266803996927</v>
-      </c>
-      <c r="J9">
-        <v>337.8565424043752</v>
-      </c>
-      <c r="K9">
-        <v>490.7017127893808</v>
-      </c>
-      <c r="L9">
-        <v>186.7731896856224</v>
-      </c>
-      <c r="M9">
-        <v>1010.927313910028</v>
-      </c>
-      <c r="N9">
-        <v>60.91298156209996</v>
-      </c>
-      <c r="O9">
-        <v>1134.052754441961</v>
-      </c>
-      <c r="P9">
-        <v>1165.811067471609</v>
-      </c>
-      <c r="Q9">
-        <v>459.1784902316442</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1020.552414202997</v>
-      </c>
-      <c r="C10">
-        <v>912.0535771003205</v>
-      </c>
-      <c r="D10">
-        <v>666.0138534315852</v>
-      </c>
-      <c r="E10">
-        <v>1240.579484548476</v>
-      </c>
-      <c r="F10">
-        <v>1232.486829395339</v>
-      </c>
-      <c r="G10">
-        <v>385.6563866052977</v>
-      </c>
-      <c r="H10">
-        <v>641.9594852595951</v>
-      </c>
-      <c r="I10">
-        <v>965.3562005878729</v>
-      </c>
-      <c r="J10">
-        <v>398.5652957564151</v>
-      </c>
-      <c r="K10">
-        <v>308.9022872069615</v>
-      </c>
-      <c r="L10">
-        <v>144.5733661984407</v>
-      </c>
-      <c r="M10">
-        <v>997.841651850218</v>
-      </c>
-      <c r="N10">
-        <v>190.1294298552628</v>
-      </c>
-      <c r="O10">
-        <v>170.0100131541906</v>
-      </c>
-      <c r="P10">
-        <v>196.7193925936567</v>
-      </c>
-      <c r="Q10">
-        <v>908.5565906338715</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>638.4432120319192</v>
-      </c>
-      <c r="C11">
-        <v>815.2458727442865</v>
-      </c>
-      <c r="D11">
-        <v>401.8755198091228</v>
-      </c>
-      <c r="E11">
-        <v>512.7523495349006</v>
-      </c>
-      <c r="F11">
-        <v>24.18403768123348</v>
-      </c>
-      <c r="G11">
-        <v>49.67651197350349</v>
-      </c>
-      <c r="H11">
-        <v>917.2401665724678</v>
-      </c>
-      <c r="I11">
-        <v>521.6107595226214</v>
-      </c>
-      <c r="J11">
-        <v>1033.683624394257</v>
-      </c>
-      <c r="K11">
-        <v>353.1028855262384</v>
-      </c>
-      <c r="L11">
-        <v>286.3153821831762</v>
-      </c>
-      <c r="M11">
-        <v>997.633843895895</v>
-      </c>
-      <c r="N11">
-        <v>1118.474860929914</v>
-      </c>
-      <c r="O11">
-        <v>216.3762918427473</v>
-      </c>
-      <c r="P11">
-        <v>688.3907649338015</v>
-      </c>
-      <c r="Q11">
-        <v>739.4431324120172</v>
+        <v>30.51883919435085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>